<commit_message>
6 lesson Done HW
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="19">
   <si>
     <t xml:space="preserve"> № </t>
   </si>
@@ -554,7 +554,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1059,6 +1059,468 @@
         <v>44086.82228727</v>
       </c>
     </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="2">
+        <v>44087.81463707585</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2">
+        <v>44087.81464879269</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="E37" s="2">
+        <v>44087.81464881967</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="2">
+        <v>44087.81464897447</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2">
+        <v>44087.81465225227</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="2">
+        <v>44087.81465226878</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2">
+        <v>44087.81465229909</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1</v>
+      </c>
+      <c r="E42" s="2">
+        <v>44087.81465525642</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+      <c r="E43" s="2">
+        <v>44087.81465527238</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2">
+        <v>44087.81465529553</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="2">
+        <v>44087.81465877905</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+      <c r="E46" s="2">
+        <v>44087.81465879554</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="2">
+        <v>44087.81465881842</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="2">
+        <v>44087.81466267136</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" s="2">
+        <v>44087.81466269307</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="2">
+        <v>44087.81466271514</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2">
+        <v>44087.81466556362</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="E52" s="2">
+        <v>44087.81466557922</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1</v>
+      </c>
+      <c r="E53" s="2">
+        <v>44087.81466560782</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
+      <c r="E54" s="2">
+        <v>44087.81466854236</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+      <c r="E55" s="2">
+        <v>44087.81466855935</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="E56" s="2">
+        <v>44087.81466858118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1</v>
+      </c>
+      <c r="E57" s="2">
+        <v>44087.81467160763</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1</v>
+      </c>
+      <c r="E58" s="2">
+        <v>44087.8146716242</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1</v>
+      </c>
+      <c r="E59" s="2">
+        <v>44087.81467164343</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1</v>
+      </c>
+      <c r="E60" s="2">
+        <v>44087.81467425697</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1</v>
+      </c>
+      <c r="E61" s="2">
+        <v>44087.81467427583</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="3">
+        <v>1</v>
+      </c>
+      <c r="E62" s="2">
+        <v>44087.81467433368</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="1">
+        <v>1</v>
+      </c>
+      <c r="E63" s="2">
+        <v>44087.81467437302</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="3">
+        <v>1</v>
+      </c>
+      <c r="E64" s="2">
+        <v>44087.81467439864</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="1">
+        <v>1</v>
+      </c>
+      <c r="E65" s="2">
+        <v>44087.81467441384</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>16</v>
+      </c>
+      <c r="D66" s="3">
+        <v>1</v>
+      </c>
+      <c r="E66" s="2">
+        <v>44087.81467443667</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="1">
+        <v>1</v>
+      </c>
+      <c r="E67" s="2">
+        <v>44087.81467445286</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>